<commit_message>
fix old, broken, model-based validation
</commit_message>
<xml_diff>
--- a/tests/060_simple.xlsx
+++ b/tests/060_simple.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/Work/rdflib/VocExcel/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9B0F7E-E6D5-9947-BE51-8724A23CA19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{719F51F7-9A0B-EA42-9D1D-871075496227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1700" yWindow="500" windowWidth="36700" windowHeight="21100" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -190,9 +190,6 @@
   </si>
   <si>
     <t>Optional: an IRI if you have one, else just a name</t>
-  </si>
-  <si>
-    <t>0.5.0</t>
   </si>
   <si>
     <t>VocExcel</t>
@@ -809,6 +806,9 @@
   <si>
     <t>http://www.w3.org/2004/02/skos/core#</t>
   </si>
+  <si>
+    <t>0.6.0</t>
+  </si>
 </sst>
 </file>
 
@@ -817,17 +817,10 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -859,13 +852,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="50"/>
@@ -1006,18 +992,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor theme="0"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1058,43 +1038,40 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1102,143 +1079,100 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1250,44 +1184,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFB47CFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1501,167 +1448,125 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K990"/>
+  <dimension ref="B1:E983"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A8" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.25" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.25" style="13"/>
-    <col min="2" max="2" width="59.625" style="14" customWidth="1"/>
-    <col min="3" max="3" width="12.25" style="13"/>
-    <col min="4" max="4" width="23.75" style="14" customWidth="1"/>
-    <col min="5" max="9" width="12.25" style="13"/>
-    <col min="10" max="10" width="21.125" style="13" customWidth="1"/>
-    <col min="11" max="24" width="12.25" style="13"/>
-    <col min="25" max="25" width="12.25" style="13" customWidth="1"/>
-    <col min="26" max="26" width="9.5" style="13" customWidth="1"/>
-    <col min="27" max="16384" width="12.25" style="13"/>
+    <col min="1" max="1" width="12.25" style="12"/>
+    <col min="2" max="2" width="59.625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="12.25" style="12"/>
+    <col min="4" max="4" width="23.75" style="13" customWidth="1"/>
+    <col min="5" max="9" width="12.25" style="12"/>
+    <col min="10" max="10" width="21.125" style="12" customWidth="1"/>
+    <col min="11" max="24" width="12.25" style="12"/>
+    <col min="25" max="25" width="12.25" style="12" customWidth="1"/>
+    <col min="26" max="26" width="9.5" style="12" customWidth="1"/>
+    <col min="27" max="16384" width="12.25" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="12"/>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-    </row>
-    <row r="2" spans="1:11" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="12"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-    </row>
-    <row r="3" spans="1:11" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="K3" s="12"/>
-    </row>
-    <row r="4" spans="1:11" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="12"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="K4" s="12"/>
-    </row>
-    <row r="5" spans="1:11" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:11" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:11" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="15" t="s">
+    <row r="1" spans="2:5" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" ht="18" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="2:5" ht="13" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="2:5" ht="38" x14ac:dyDescent="0.2">
+      <c r="B4" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="D5" s="12"/>
+    </row>
+    <row r="6" spans="2:5" ht="38" x14ac:dyDescent="0.2">
+      <c r="B6" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="54" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="B7" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="12"/>
+    </row>
+    <row r="8" spans="2:5" ht="38" x14ac:dyDescent="0.2">
+      <c r="B8" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="54" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="B9" s="53"/>
+    </row>
+    <row r="10" spans="2:5" ht="38" x14ac:dyDescent="0.2">
+      <c r="B10" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="13" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="18" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:11" ht="18" x14ac:dyDescent="0.2">
-      <c r="B11" s="16" t="s">
+      <c r="E10" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="18" x14ac:dyDescent="0.2">
-      <c r="D12" s="13"/>
-    </row>
-    <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.2">
-      <c r="B13" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="19" x14ac:dyDescent="0.2">
-      <c r="B14" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="D14" s="13"/>
-    </row>
-    <row r="15" spans="1:11" ht="19" x14ac:dyDescent="0.2">
-      <c r="B15" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="18" x14ac:dyDescent="0.2">
-      <c r="B16" s="19"/>
-    </row>
-    <row r="17" spans="2:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="16" t="s">
+    </row>
+    <row r="11" spans="2:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="D11" s="12"/>
+    </row>
+    <row r="12" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="D18" s="13"/>
-    </row>
-    <row r="19" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="16" t="s">
+      <c r="D12" s="12"/>
+    </row>
+    <row r="13" spans="2:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="B13" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="D19" s="13"/>
-    </row>
-    <row r="20" spans="2:5" ht="19" x14ac:dyDescent="0.2">
-      <c r="B20" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="D20" s="13"/>
-    </row>
-    <row r="21" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="D21" s="13"/>
-    </row>
-    <row r="22" spans="2:5" ht="18" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="2:5" ht="18" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="2:5" ht="18" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="2:5" ht="18" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="2:5" ht="18" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="2:5" ht="18" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="2:5" ht="18" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="2:5" ht="18" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="2:5" ht="18" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="2:5" ht="18" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="2:5" ht="18" x14ac:dyDescent="0.2"/>
+      <c r="D13" s="12"/>
+    </row>
+    <row r="14" spans="2:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="D14" s="12"/>
+    </row>
+    <row r="15" spans="2:5" ht="18" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="2:5" ht="18" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="18" x14ac:dyDescent="0.2"/>
+    <row r="18" ht="18" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="18" x14ac:dyDescent="0.2"/>
+    <row r="20" ht="18" x14ac:dyDescent="0.2"/>
+    <row r="21" ht="18" x14ac:dyDescent="0.2"/>
+    <row r="22" ht="18" x14ac:dyDescent="0.2"/>
+    <row r="23" ht="18" x14ac:dyDescent="0.2"/>
+    <row r="24" ht="18" x14ac:dyDescent="0.2"/>
+    <row r="25" ht="18" x14ac:dyDescent="0.2"/>
+    <row r="26" ht="18" x14ac:dyDescent="0.2"/>
+    <row r="27" ht="18" x14ac:dyDescent="0.2"/>
+    <row r="28" ht="18" x14ac:dyDescent="0.2"/>
+    <row r="29" ht="18" x14ac:dyDescent="0.2"/>
+    <row r="30" ht="18" x14ac:dyDescent="0.2"/>
+    <row r="31" ht="18" x14ac:dyDescent="0.2"/>
+    <row r="32" ht="18" x14ac:dyDescent="0.2"/>
     <row r="33" ht="18" x14ac:dyDescent="0.2"/>
     <row r="34" ht="18" x14ac:dyDescent="0.2"/>
     <row r="35" ht="18" x14ac:dyDescent="0.2"/>
@@ -2613,35 +2518,14 @@
     <row r="981" ht="18" x14ac:dyDescent="0.2"/>
     <row r="982" ht="18" x14ac:dyDescent="0.2"/>
     <row r="983" ht="18" x14ac:dyDescent="0.2"/>
-    <row r="984" ht="18" x14ac:dyDescent="0.2"/>
-    <row r="985" ht="18" x14ac:dyDescent="0.2"/>
-    <row r="986" ht="18" x14ac:dyDescent="0.2"/>
-    <row r="987" ht="18" x14ac:dyDescent="0.2"/>
-    <row r="988" ht="18" x14ac:dyDescent="0.2"/>
-    <row r="989" ht="18" x14ac:dyDescent="0.2"/>
-    <row r="990" ht="18" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B1:G2"/>
-  </mergeCells>
-  <conditionalFormatting sqref="H1:J2 A1:G4 K1:K4">
-    <cfRule type="containsBlanks" dxfId="1" priority="9">
-      <formula>LEN(TRIM(A1))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K1:K4">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="10">
-      <formula>LEN(TRIM(K1))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E17" r:id="rId1" location="contact" xr:uid="{5574247B-F7EF-F747-9C78-D6AB2FDE5EF7}"/>
-    <hyperlink ref="E13" r:id="rId2" xr:uid="{E4837409-9B33-4A40-A996-49AC2E8A520E}"/>
-    <hyperlink ref="E15" r:id="rId3" xr:uid="{3F460BC4-66C6-3F42-B263-B8D5327080BF}"/>
-    <hyperlink ref="B20" r:id="rId4" xr:uid="{DB01703C-A595-564D-90B4-3729255150D8}"/>
-    <hyperlink ref="B14" r:id="rId5" xr:uid="{0725B119-35B4-E04C-88B9-B8862A83A97E}"/>
-    <hyperlink ref="B15" r:id="rId6" xr:uid="{895C0FE1-98FA-0F43-9D17-D170E5EFDE7A}"/>
+    <hyperlink ref="E10" r:id="rId1" location="contact" xr:uid="{5574247B-F7EF-F747-9C78-D6AB2FDE5EF7}"/>
+    <hyperlink ref="E6" r:id="rId2" xr:uid="{E4837409-9B33-4A40-A996-49AC2E8A520E}"/>
+    <hyperlink ref="E8" r:id="rId3" xr:uid="{3F460BC4-66C6-3F42-B263-B8D5327080BF}"/>
+    <hyperlink ref="B13" r:id="rId4" xr:uid="{DB01703C-A595-564D-90B4-3729255150D8}"/>
+    <hyperlink ref="B7" r:id="rId5" xr:uid="{0725B119-35B4-E04C-88B9-B8862A83A97E}"/>
+    <hyperlink ref="B8" r:id="rId6" xr:uid="{895C0FE1-98FA-0F43-9D17-D170E5EFDE7A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2651,13 +2535,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E056D66-684B-EA44-9D39-98A26FD38952}">
   <dimension ref="A2:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.75" style="20" customWidth="1"/>
+    <col min="1" max="1" width="26.75" style="16" customWidth="1"/>
     <col min="2" max="2" width="108.125" style="4" customWidth="1"/>
     <col min="3" max="3" width="59.75" style="6" customWidth="1"/>
     <col min="4" max="16384" width="10.625" style="4"/>
@@ -2665,61 +2549,61 @@
   <sheetData>
     <row r="2" spans="1:3" ht="63" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="171" x14ac:dyDescent="0.2">
+      <c r="A3" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="269" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="173" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="97" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="11"/>
+    </row>
+    <row r="7" spans="1:3" ht="78" x14ac:dyDescent="0.2">
+      <c r="A7" s="17"/>
+      <c r="B7" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="8"/>
+    </row>
+    <row r="8" spans="1:3" ht="38" x14ac:dyDescent="0.2">
+      <c r="A8" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="171" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="269" x14ac:dyDescent="0.2">
-      <c r="A4" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="173" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="97" x14ac:dyDescent="0.2">
-      <c r="A6" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C6" s="11"/>
-    </row>
-    <row r="7" spans="1:3" ht="78" x14ac:dyDescent="0.2">
-      <c r="A7" s="21"/>
-      <c r="B7" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="8"/>
-    </row>
-    <row r="8" spans="1:3" ht="38" x14ac:dyDescent="0.2">
-      <c r="A8" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="C8" s="3"/>
     </row>
@@ -2728,11 +2612,11 @@
       <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:3" ht="57" x14ac:dyDescent="0.2">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10" s="4"/>
     </row>
@@ -2741,11 +2625,11 @@
       <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:3" ht="42" x14ac:dyDescent="0.2">
-      <c r="A12" s="20" t="s">
-        <v>44</v>
+      <c r="A12" s="16" t="s">
+        <v>43</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" s="3"/>
     </row>
@@ -2754,11 +2638,11 @@
       <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:3" ht="38" x14ac:dyDescent="0.2">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" s="3"/>
     </row>
@@ -2767,11 +2651,11 @@
       <c r="C15" s="3"/>
     </row>
     <row r="16" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
-        <v>43</v>
+      <c r="A16" s="16" t="s">
+        <v>42</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C16" s="3"/>
     </row>
@@ -2804,164 +2688,164 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="25" x14ac:dyDescent="0.2">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-    </row>
-    <row r="2" spans="1:4" s="45" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="35" t="s">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+    </row>
+    <row r="2" spans="1:4" s="41" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="44" t="s">
-        <v>99</v>
-      </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="39" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="44" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="60" t="s">
-        <v>120</v>
-      </c>
-      <c r="C3" s="43" t="s">
-        <v>91</v>
-      </c>
-      <c r="D3" s="43" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="61" t="s">
-        <v>121</v>
-      </c>
-      <c r="C4" s="43" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="43" t="s">
+      <c r="D5" s="39" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="61" t="s">
+    <row r="6" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="46">
+        <v>44896</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="46">
+        <v>44896</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="45" t="s">
         <v>122</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C8" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="39" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="47" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="39" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="C11" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="D5" s="43" t="s">
+      <c r="D11" s="39" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="62">
-        <v>44896</v>
-      </c>
-      <c r="C6" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="43" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="62">
-        <v>44896</v>
-      </c>
-      <c r="C7" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="43" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="61" t="s">
-        <v>123</v>
-      </c>
-      <c r="C8" s="43" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="43" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="60" t="s">
-        <v>124</v>
-      </c>
-      <c r="C9" s="43" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="43" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="63" t="s">
-        <v>125</v>
-      </c>
-      <c r="C10" s="43" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="43" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="64" t="s">
-        <v>126</v>
-      </c>
-      <c r="C11" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="D11" s="43" t="s">
-        <v>3</v>
-      </c>
-    </row>
     <row r="12" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="61" t="s">
-        <v>123</v>
-      </c>
-      <c r="C12" s="43" t="s">
+      <c r="B12" s="45" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="43" t="s">
+      <c r="D12" s="39" t="s">
         <v>31</v>
       </c>
     </row>
@@ -5946,139 +5830,148 @@
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="49" style="25" customWidth="1"/>
-    <col min="2" max="2" width="27.5" style="25" customWidth="1"/>
-    <col min="3" max="3" width="55.25" style="26" customWidth="1"/>
-    <col min="4" max="4" width="20.625" style="26" customWidth="1"/>
-    <col min="5" max="5" width="44.625" style="26" customWidth="1"/>
-    <col min="6" max="7" width="26.625" style="26" customWidth="1"/>
-    <col min="8" max="8" width="22" style="26" customWidth="1"/>
-    <col min="9" max="16384" width="10.625" style="25"/>
+    <col min="1" max="1" width="49" style="21" customWidth="1"/>
+    <col min="2" max="2" width="27.5" style="21" customWidth="1"/>
+    <col min="3" max="3" width="55.25" style="22" customWidth="1"/>
+    <col min="4" max="4" width="20.625" style="22" customWidth="1"/>
+    <col min="5" max="5" width="44.625" style="22" customWidth="1"/>
+    <col min="6" max="7" width="26.625" style="22" customWidth="1"/>
+    <col min="8" max="8" width="22" style="22" customWidth="1"/>
+    <col min="9" max="16384" width="10.625" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
     </row>
     <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.2">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2" s="38" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="98" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="F2" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="42" t="s">
-        <v>92</v>
-      </c>
-      <c r="H2" s="42" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="98" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" s="30" t="s">
+      <c r="E3" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="D3" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="E3" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="F3" s="31" t="s">
+      <c r="G3" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="G3" s="31" t="s">
+      <c r="H3" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="H3" s="31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="19" x14ac:dyDescent="0.2">
-      <c r="A4" s="57" t="s">
+    </row>
+    <row r="4" spans="1:8" s="64" customFormat="1" ht="38" x14ac:dyDescent="0.2">
+      <c r="A4" s="62" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="B4" s="56" t="s">
+      <c r="C4" s="65" t="s">
         <v>109</v>
       </c>
-      <c r="C4" s="57" t="s">
+      <c r="D4" s="63"/>
+      <c r="E4" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="E4" s="58" t="s">
+      <c r="F4" s="63"/>
+      <c r="G4" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="H4" s="63"/>
+    </row>
+    <row r="5" spans="1:8" s="64" customFormat="1" ht="38" x14ac:dyDescent="0.2">
+      <c r="A5" s="62" t="s">
         <v>111</v>
       </c>
-      <c r="G4" s="26" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="38" x14ac:dyDescent="0.2">
-      <c r="A5" s="57" t="s">
+      <c r="B5" s="62" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="65" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="B5" s="57" t="s">
-        <v>114</v>
-      </c>
-      <c r="C5" s="57" t="s">
+      <c r="G5" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="H5" s="63"/>
+    </row>
+    <row r="6" spans="1:8" s="64" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+      <c r="A6" s="62" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="F5" s="58" t="s">
-        <v>113</v>
-      </c>
-      <c r="G5" s="59" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="57" x14ac:dyDescent="0.2">
-      <c r="A6" s="57" t="s">
-        <v>111</v>
-      </c>
-      <c r="B6" s="56" t="s">
-        <v>118</v>
-      </c>
-      <c r="C6" s="58" t="s">
-        <v>117</v>
-      </c>
-      <c r="D6" s="58" t="s">
-        <v>116</v>
-      </c>
-      <c r="F6" s="58"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="56"/>
+      <c r="B7" s="43"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="56"/>
+      <c r="A13" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6086,6 +5979,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{368B2852-A514-F844-8732-8A4C6C92ECF9}"/>
+    <hyperlink ref="G4" r:id="rId2" xr:uid="{9520918D-7210-FF4E-9776-B7067D875568}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6105,98 +5999,98 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.25" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.25" style="40" customWidth="1"/>
-    <col min="2" max="6" width="25" style="24" customWidth="1"/>
-    <col min="7" max="7" width="21.125" style="24" customWidth="1"/>
-    <col min="8" max="8" width="24.5" style="24" customWidth="1"/>
-    <col min="9" max="16384" width="12.25" style="23"/>
+    <col min="1" max="1" width="33.25" style="36" customWidth="1"/>
+    <col min="2" max="6" width="25" style="20" customWidth="1"/>
+    <col min="7" max="7" width="21.125" style="20" customWidth="1"/>
+    <col min="8" max="8" width="24.5" style="20" customWidth="1"/>
+    <col min="9" max="16384" width="12.25" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="52" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
+      <c r="A1" s="58" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
     </row>
     <row r="2" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="D2" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="G2" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="H2" s="32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" s="30" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="29"/>
+      <c r="T3" s="29"/>
+      <c r="U3" s="29"/>
+      <c r="V3" s="29"/>
+      <c r="W3" s="29"/>
+      <c r="X3" s="29"/>
+      <c r="Y3" s="29"/>
+      <c r="Z3" s="29"/>
+      <c r="AA3" s="29"/>
+    </row>
+    <row r="4" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="G2" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="H2" s="36" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" s="34" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="38" t="s">
-        <v>89</v>
-      </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="37" t="s">
-        <v>88</v>
-      </c>
-      <c r="H3" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="33"/>
-      <c r="R3" s="33"/>
-      <c r="S3" s="33"/>
-      <c r="T3" s="33"/>
-      <c r="U3" s="33"/>
-      <c r="V3" s="33"/>
-      <c r="W3" s="33"/>
-      <c r="X3" s="33"/>
-      <c r="Y3" s="33"/>
-      <c r="Z3" s="33"/>
-      <c r="AA3" s="33"/>
-    </row>
-    <row r="4" spans="1:27" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="65" t="s">
-        <v>108</v>
-      </c>
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="51" t="s">
+        <v>128</v>
+      </c>
+      <c r="G4" s="50" t="s">
+        <v>127</v>
+      </c>
+      <c r="H4" s="51" t="s">
         <v>129</v>
-      </c>
-      <c r="G4" s="66" t="s">
-        <v>128</v>
-      </c>
-      <c r="H4" s="67" t="s">
-        <v>130</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -6244,1424 +6138,1424 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.25" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.75" style="24" customWidth="1"/>
-    <col min="2" max="2" width="23.5" style="24" customWidth="1"/>
-    <col min="3" max="3" width="47.625" style="24" customWidth="1"/>
-    <col min="4" max="4" width="45.25" style="24" customWidth="1"/>
-    <col min="5" max="5" width="26.125" style="24" customWidth="1"/>
-    <col min="6" max="16384" width="12.25" style="23"/>
+    <col min="1" max="1" width="33.75" style="20" customWidth="1"/>
+    <col min="2" max="2" width="23.5" style="20" customWidth="1"/>
+    <col min="3" max="3" width="47.625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="45.25" style="20" customWidth="1"/>
+    <col min="5" max="5" width="26.125" style="20" customWidth="1"/>
+    <col min="6" max="16384" width="12.25" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
     </row>
     <row r="2" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="32" t="s">
-        <v>96</v>
-      </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="28" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="46" t="s">
-        <v>105</v>
-      </c>
-      <c r="E3" s="32"/>
-    </row>
-    <row r="4" spans="1:5" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="26" t="s">
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="E3" s="28"/>
+    </row>
+    <row r="4" spans="1:5" s="21" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="C4" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="C4" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="D4" s="26" t="s">
+      <c r="E4" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="E4" s="26" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="25" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
+    </row>
+    <row r="5" spans="1:5" s="21" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="39"/>
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="39"/>
+      <c r="A7" s="35"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="35"/>
     </row>
     <row r="8" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="39"/>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="39"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="35"/>
     </row>
     <row r="9" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="39"/>
-      <c r="B9" s="39"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="39"/>
+      <c r="A9" s="35"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="35"/>
     </row>
     <row r="10" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="39"/>
-      <c r="B10" s="39"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="39"/>
+      <c r="A10" s="35"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="35"/>
     </row>
     <row r="11" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="39"/>
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="39"/>
+      <c r="A11" s="35"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="35"/>
     </row>
     <row r="12" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="39"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="39"/>
+      <c r="A12" s="35"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="35"/>
     </row>
     <row r="13" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="39"/>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
+      <c r="A13" s="35"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
     </row>
     <row r="14" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="39"/>
-      <c r="B14" s="39"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
+      <c r="A14" s="35"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
     </row>
     <row r="15" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="39"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
+      <c r="A15" s="35"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
     </row>
     <row r="16" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="39"/>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
     </row>
     <row r="17" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="39"/>
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
     </row>
     <row r="18" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="39"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
     </row>
     <row r="19" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="39"/>
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
     </row>
     <row r="20" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="39"/>
-      <c r="B20" s="39"/>
-      <c r="C20" s="39"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="39"/>
+      <c r="A20" s="35"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
     </row>
     <row r="21" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="39"/>
-      <c r="B21" s="39"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="39"/>
+      <c r="A21" s="35"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
     </row>
     <row r="22" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="39"/>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
+      <c r="A22" s="35"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="35"/>
     </row>
     <row r="23" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="39"/>
-      <c r="B23" s="39"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
+      <c r="A23" s="35"/>
+      <c r="B23" s="35"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
     </row>
     <row r="24" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="39"/>
-      <c r="B24" s="39"/>
-      <c r="C24" s="39"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="39"/>
+      <c r="A24" s="35"/>
+      <c r="B24" s="35"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
     </row>
     <row r="25" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="39"/>
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="39"/>
+      <c r="A25" s="35"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
     </row>
     <row r="26" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="39"/>
-      <c r="B26" s="39"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
+      <c r="A26" s="35"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
     </row>
     <row r="27" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="39"/>
-      <c r="B27" s="39"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
+      <c r="A27" s="35"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
     </row>
     <row r="28" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="39"/>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
+      <c r="A28" s="35"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
     </row>
     <row r="29" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="39"/>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
+      <c r="A29" s="35"/>
+      <c r="B29" s="35"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
     </row>
     <row r="30" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="39"/>
-      <c r="B30" s="39"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
+      <c r="A30" s="35"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="35"/>
     </row>
     <row r="31" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="39"/>
-      <c r="B31" s="39"/>
-      <c r="C31" s="39"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="39"/>
+      <c r="A31" s="35"/>
+      <c r="B31" s="35"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="35"/>
     </row>
     <row r="32" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="39"/>
-      <c r="B32" s="39"/>
-      <c r="C32" s="39"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="39"/>
+      <c r="A32" s="35"/>
+      <c r="B32" s="35"/>
+      <c r="C32" s="35"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
     </row>
     <row r="33" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="39"/>
-      <c r="B33" s="39"/>
-      <c r="C33" s="39"/>
-      <c r="D33" s="39"/>
-      <c r="E33" s="39"/>
+      <c r="A33" s="35"/>
+      <c r="B33" s="35"/>
+      <c r="C33" s="35"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="35"/>
     </row>
     <row r="34" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="39"/>
-      <c r="B34" s="39"/>
-      <c r="C34" s="39"/>
-      <c r="D34" s="39"/>
-      <c r="E34" s="39"/>
+      <c r="A34" s="35"/>
+      <c r="B34" s="35"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
     </row>
     <row r="35" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="39"/>
-      <c r="B35" s="39"/>
-      <c r="C35" s="39"/>
-      <c r="D35" s="39"/>
-      <c r="E35" s="39"/>
+      <c r="A35" s="35"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
     </row>
     <row r="36" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="39"/>
-      <c r="B36" s="39"/>
-      <c r="C36" s="39"/>
-      <c r="D36" s="39"/>
-      <c r="E36" s="39"/>
+      <c r="A36" s="35"/>
+      <c r="B36" s="35"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="35"/>
     </row>
     <row r="37" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="39"/>
-      <c r="B37" s="39"/>
-      <c r="C37" s="39"/>
-      <c r="D37" s="39"/>
-      <c r="E37" s="39"/>
+      <c r="A37" s="35"/>
+      <c r="B37" s="35"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="35"/>
     </row>
     <row r="38" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="39"/>
-      <c r="B38" s="39"/>
-      <c r="C38" s="39"/>
-      <c r="D38" s="39"/>
-      <c r="E38" s="39"/>
+      <c r="A38" s="35"/>
+      <c r="B38" s="35"/>
+      <c r="C38" s="35"/>
+      <c r="D38" s="35"/>
+      <c r="E38" s="35"/>
     </row>
     <row r="39" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="39"/>
-      <c r="B39" s="39"/>
-      <c r="C39" s="39"/>
-      <c r="D39" s="39"/>
-      <c r="E39" s="39"/>
+      <c r="A39" s="35"/>
+      <c r="B39" s="35"/>
+      <c r="C39" s="35"/>
+      <c r="D39" s="35"/>
+      <c r="E39" s="35"/>
     </row>
     <row r="40" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="39"/>
-      <c r="B40" s="39"/>
-      <c r="C40" s="39"/>
-      <c r="D40" s="39"/>
-      <c r="E40" s="39"/>
+      <c r="A40" s="35"/>
+      <c r="B40" s="35"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="35"/>
     </row>
     <row r="41" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="39"/>
-      <c r="B41" s="39"/>
-      <c r="C41" s="39"/>
-      <c r="D41" s="39"/>
-      <c r="E41" s="39"/>
+      <c r="A41" s="35"/>
+      <c r="B41" s="35"/>
+      <c r="C41" s="35"/>
+      <c r="D41" s="35"/>
+      <c r="E41" s="35"/>
     </row>
     <row r="42" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="39"/>
-      <c r="B42" s="39"/>
-      <c r="C42" s="39"/>
-      <c r="D42" s="39"/>
-      <c r="E42" s="39"/>
+      <c r="A42" s="35"/>
+      <c r="B42" s="35"/>
+      <c r="C42" s="35"/>
+      <c r="D42" s="35"/>
+      <c r="E42" s="35"/>
     </row>
     <row r="43" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="39"/>
-      <c r="B43" s="39"/>
-      <c r="C43" s="39"/>
-      <c r="D43" s="39"/>
-      <c r="E43" s="39"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
+      <c r="C43" s="35"/>
+      <c r="D43" s="35"/>
+      <c r="E43" s="35"/>
     </row>
     <row r="44" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="39"/>
-      <c r="B44" s="39"/>
-      <c r="C44" s="39"/>
-      <c r="D44" s="39"/>
-      <c r="E44" s="39"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
+      <c r="C44" s="35"/>
+      <c r="D44" s="35"/>
+      <c r="E44" s="35"/>
     </row>
     <row r="45" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="39"/>
-      <c r="B45" s="39"/>
-      <c r="C45" s="39"/>
-      <c r="D45" s="39"/>
-      <c r="E45" s="39"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
+      <c r="C45" s="35"/>
+      <c r="D45" s="35"/>
+      <c r="E45" s="35"/>
     </row>
     <row r="46" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="39"/>
-      <c r="B46" s="39"/>
-      <c r="C46" s="39"/>
-      <c r="D46" s="39"/>
-      <c r="E46" s="39"/>
+      <c r="A46" s="35"/>
+      <c r="B46" s="35"/>
+      <c r="C46" s="35"/>
+      <c r="D46" s="35"/>
+      <c r="E46" s="35"/>
     </row>
     <row r="47" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="39"/>
-      <c r="B47" s="39"/>
-      <c r="C47" s="39"/>
-      <c r="D47" s="39"/>
-      <c r="E47" s="39"/>
+      <c r="A47" s="35"/>
+      <c r="B47" s="35"/>
+      <c r="C47" s="35"/>
+      <c r="D47" s="35"/>
+      <c r="E47" s="35"/>
     </row>
     <row r="48" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="39"/>
-      <c r="B48" s="39"/>
-      <c r="C48" s="39"/>
-      <c r="D48" s="39"/>
-      <c r="E48" s="39"/>
+      <c r="A48" s="35"/>
+      <c r="B48" s="35"/>
+      <c r="C48" s="35"/>
+      <c r="D48" s="35"/>
+      <c r="E48" s="35"/>
     </row>
     <row r="49" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="39"/>
-      <c r="B49" s="39"/>
-      <c r="C49" s="39"/>
-      <c r="D49" s="39"/>
-      <c r="E49" s="39"/>
+      <c r="A49" s="35"/>
+      <c r="B49" s="35"/>
+      <c r="C49" s="35"/>
+      <c r="D49" s="35"/>
+      <c r="E49" s="35"/>
     </row>
     <row r="50" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="39"/>
-      <c r="B50" s="39"/>
-      <c r="C50" s="39"/>
-      <c r="D50" s="39"/>
-      <c r="E50" s="39"/>
+      <c r="A50" s="35"/>
+      <c r="B50" s="35"/>
+      <c r="C50" s="35"/>
+      <c r="D50" s="35"/>
+      <c r="E50" s="35"/>
     </row>
     <row r="51" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="39"/>
-      <c r="B51" s="39"/>
-      <c r="C51" s="39"/>
-      <c r="D51" s="39"/>
-      <c r="E51" s="39"/>
+      <c r="A51" s="35"/>
+      <c r="B51" s="35"/>
+      <c r="C51" s="35"/>
+      <c r="D51" s="35"/>
+      <c r="E51" s="35"/>
     </row>
     <row r="52" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="39"/>
-      <c r="B52" s="39"/>
-      <c r="C52" s="39"/>
-      <c r="D52" s="39"/>
-      <c r="E52" s="39"/>
+      <c r="A52" s="35"/>
+      <c r="B52" s="35"/>
+      <c r="C52" s="35"/>
+      <c r="D52" s="35"/>
+      <c r="E52" s="35"/>
     </row>
     <row r="53" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="39"/>
-      <c r="B53" s="39"/>
-      <c r="C53" s="39"/>
-      <c r="D53" s="39"/>
-      <c r="E53" s="39"/>
+      <c r="A53" s="35"/>
+      <c r="B53" s="35"/>
+      <c r="C53" s="35"/>
+      <c r="D53" s="35"/>
+      <c r="E53" s="35"/>
     </row>
     <row r="54" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="39"/>
-      <c r="B54" s="39"/>
-      <c r="C54" s="39"/>
-      <c r="D54" s="39"/>
-      <c r="E54" s="39"/>
+      <c r="A54" s="35"/>
+      <c r="B54" s="35"/>
+      <c r="C54" s="35"/>
+      <c r="D54" s="35"/>
+      <c r="E54" s="35"/>
     </row>
     <row r="55" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="39"/>
-      <c r="B55" s="39"/>
-      <c r="C55" s="39"/>
-      <c r="D55" s="39"/>
-      <c r="E55" s="39"/>
+      <c r="A55" s="35"/>
+      <c r="B55" s="35"/>
+      <c r="C55" s="35"/>
+      <c r="D55" s="35"/>
+      <c r="E55" s="35"/>
     </row>
     <row r="56" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="39"/>
-      <c r="B56" s="39"/>
-      <c r="C56" s="39"/>
-      <c r="D56" s="39"/>
-      <c r="E56" s="39"/>
+      <c r="A56" s="35"/>
+      <c r="B56" s="35"/>
+      <c r="C56" s="35"/>
+      <c r="D56" s="35"/>
+      <c r="E56" s="35"/>
     </row>
     <row r="57" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="39"/>
-      <c r="B57" s="39"/>
-      <c r="C57" s="39"/>
-      <c r="D57" s="39"/>
-      <c r="E57" s="39"/>
+      <c r="A57" s="35"/>
+      <c r="B57" s="35"/>
+      <c r="C57" s="35"/>
+      <c r="D57" s="35"/>
+      <c r="E57" s="35"/>
     </row>
     <row r="58" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="39"/>
-      <c r="B58" s="39"/>
-      <c r="C58" s="39"/>
-      <c r="D58" s="39"/>
-      <c r="E58" s="39"/>
+      <c r="A58" s="35"/>
+      <c r="B58" s="35"/>
+      <c r="C58" s="35"/>
+      <c r="D58" s="35"/>
+      <c r="E58" s="35"/>
     </row>
     <row r="59" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="39"/>
-      <c r="B59" s="39"/>
-      <c r="C59" s="39"/>
-      <c r="D59" s="39"/>
-      <c r="E59" s="39"/>
+      <c r="A59" s="35"/>
+      <c r="B59" s="35"/>
+      <c r="C59" s="35"/>
+      <c r="D59" s="35"/>
+      <c r="E59" s="35"/>
     </row>
     <row r="60" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="39"/>
-      <c r="B60" s="39"/>
-      <c r="C60" s="39"/>
-      <c r="D60" s="39"/>
-      <c r="E60" s="39"/>
+      <c r="A60" s="35"/>
+      <c r="B60" s="35"/>
+      <c r="C60" s="35"/>
+      <c r="D60" s="35"/>
+      <c r="E60" s="35"/>
     </row>
     <row r="61" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="39"/>
-      <c r="B61" s="39"/>
-      <c r="C61" s="39"/>
-      <c r="D61" s="39"/>
-      <c r="E61" s="39"/>
+      <c r="A61" s="35"/>
+      <c r="B61" s="35"/>
+      <c r="C61" s="35"/>
+      <c r="D61" s="35"/>
+      <c r="E61" s="35"/>
     </row>
     <row r="62" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="39"/>
-      <c r="B62" s="39"/>
-      <c r="C62" s="39"/>
-      <c r="D62" s="39"/>
-      <c r="E62" s="39"/>
+      <c r="A62" s="35"/>
+      <c r="B62" s="35"/>
+      <c r="C62" s="35"/>
+      <c r="D62" s="35"/>
+      <c r="E62" s="35"/>
     </row>
     <row r="63" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="39"/>
-      <c r="B63" s="39"/>
-      <c r="C63" s="39"/>
-      <c r="D63" s="39"/>
-      <c r="E63" s="39"/>
+      <c r="A63" s="35"/>
+      <c r="B63" s="35"/>
+      <c r="C63" s="35"/>
+      <c r="D63" s="35"/>
+      <c r="E63" s="35"/>
     </row>
     <row r="64" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="39"/>
-      <c r="B64" s="39"/>
-      <c r="C64" s="39"/>
-      <c r="D64" s="39"/>
-      <c r="E64" s="39"/>
+      <c r="A64" s="35"/>
+      <c r="B64" s="35"/>
+      <c r="C64" s="35"/>
+      <c r="D64" s="35"/>
+      <c r="E64" s="35"/>
     </row>
     <row r="65" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="39"/>
-      <c r="B65" s="39"/>
-      <c r="C65" s="39"/>
-      <c r="D65" s="39"/>
-      <c r="E65" s="39"/>
+      <c r="A65" s="35"/>
+      <c r="B65" s="35"/>
+      <c r="C65" s="35"/>
+      <c r="D65" s="35"/>
+      <c r="E65" s="35"/>
     </row>
     <row r="66" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="39"/>
-      <c r="B66" s="39"/>
-      <c r="C66" s="39"/>
-      <c r="D66" s="39"/>
-      <c r="E66" s="39"/>
+      <c r="A66" s="35"/>
+      <c r="B66" s="35"/>
+      <c r="C66" s="35"/>
+      <c r="D66" s="35"/>
+      <c r="E66" s="35"/>
     </row>
     <row r="67" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="39"/>
-      <c r="B67" s="39"/>
-      <c r="C67" s="39"/>
-      <c r="D67" s="39"/>
-      <c r="E67" s="39"/>
+      <c r="A67" s="35"/>
+      <c r="B67" s="35"/>
+      <c r="C67" s="35"/>
+      <c r="D67" s="35"/>
+      <c r="E67" s="35"/>
     </row>
     <row r="68" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="39"/>
-      <c r="B68" s="39"/>
-      <c r="C68" s="39"/>
-      <c r="D68" s="39"/>
-      <c r="E68" s="39"/>
+      <c r="A68" s="35"/>
+      <c r="B68" s="35"/>
+      <c r="C68" s="35"/>
+      <c r="D68" s="35"/>
+      <c r="E68" s="35"/>
     </row>
     <row r="69" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="39"/>
-      <c r="B69" s="39"/>
-      <c r="C69" s="39"/>
-      <c r="D69" s="39"/>
-      <c r="E69" s="39"/>
+      <c r="A69" s="35"/>
+      <c r="B69" s="35"/>
+      <c r="C69" s="35"/>
+      <c r="D69" s="35"/>
+      <c r="E69" s="35"/>
     </row>
     <row r="70" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="39"/>
-      <c r="B70" s="39"/>
-      <c r="C70" s="39"/>
-      <c r="D70" s="39"/>
-      <c r="E70" s="39"/>
+      <c r="A70" s="35"/>
+      <c r="B70" s="35"/>
+      <c r="C70" s="35"/>
+      <c r="D70" s="35"/>
+      <c r="E70" s="35"/>
     </row>
     <row r="71" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="39"/>
-      <c r="B71" s="39"/>
-      <c r="C71" s="39"/>
-      <c r="D71" s="39"/>
-      <c r="E71" s="39"/>
+      <c r="A71" s="35"/>
+      <c r="B71" s="35"/>
+      <c r="C71" s="35"/>
+      <c r="D71" s="35"/>
+      <c r="E71" s="35"/>
     </row>
     <row r="72" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="39"/>
-      <c r="B72" s="39"/>
-      <c r="C72" s="39"/>
-      <c r="D72" s="39"/>
-      <c r="E72" s="39"/>
+      <c r="A72" s="35"/>
+      <c r="B72" s="35"/>
+      <c r="C72" s="35"/>
+      <c r="D72" s="35"/>
+      <c r="E72" s="35"/>
     </row>
     <row r="73" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="39"/>
-      <c r="B73" s="39"/>
-      <c r="C73" s="39"/>
-      <c r="D73" s="39"/>
-      <c r="E73" s="39"/>
+      <c r="A73" s="35"/>
+      <c r="B73" s="35"/>
+      <c r="C73" s="35"/>
+      <c r="D73" s="35"/>
+      <c r="E73" s="35"/>
     </row>
     <row r="74" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="39"/>
-      <c r="B74" s="39"/>
-      <c r="C74" s="39"/>
-      <c r="D74" s="39"/>
-      <c r="E74" s="39"/>
+      <c r="A74" s="35"/>
+      <c r="B74" s="35"/>
+      <c r="C74" s="35"/>
+      <c r="D74" s="35"/>
+      <c r="E74" s="35"/>
     </row>
     <row r="75" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="39"/>
-      <c r="B75" s="39"/>
-      <c r="C75" s="39"/>
-      <c r="D75" s="39"/>
-      <c r="E75" s="39"/>
+      <c r="A75" s="35"/>
+      <c r="B75" s="35"/>
+      <c r="C75" s="35"/>
+      <c r="D75" s="35"/>
+      <c r="E75" s="35"/>
     </row>
     <row r="76" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="39"/>
-      <c r="B76" s="39"/>
-      <c r="C76" s="39"/>
-      <c r="D76" s="39"/>
-      <c r="E76" s="39"/>
+      <c r="A76" s="35"/>
+      <c r="B76" s="35"/>
+      <c r="C76" s="35"/>
+      <c r="D76" s="35"/>
+      <c r="E76" s="35"/>
     </row>
     <row r="77" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="39"/>
-      <c r="B77" s="39"/>
-      <c r="C77" s="39"/>
-      <c r="D77" s="39"/>
-      <c r="E77" s="39"/>
+      <c r="A77" s="35"/>
+      <c r="B77" s="35"/>
+      <c r="C77" s="35"/>
+      <c r="D77" s="35"/>
+      <c r="E77" s="35"/>
     </row>
     <row r="78" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="39"/>
-      <c r="B78" s="39"/>
-      <c r="C78" s="39"/>
-      <c r="D78" s="39"/>
-      <c r="E78" s="39"/>
+      <c r="A78" s="35"/>
+      <c r="B78" s="35"/>
+      <c r="C78" s="35"/>
+      <c r="D78" s="35"/>
+      <c r="E78" s="35"/>
     </row>
     <row r="79" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="39"/>
-      <c r="B79" s="39"/>
-      <c r="C79" s="39"/>
-      <c r="D79" s="39"/>
-      <c r="E79" s="39"/>
+      <c r="A79" s="35"/>
+      <c r="B79" s="35"/>
+      <c r="C79" s="35"/>
+      <c r="D79" s="35"/>
+      <c r="E79" s="35"/>
     </row>
     <row r="80" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="39"/>
-      <c r="B80" s="39"/>
-      <c r="C80" s="39"/>
-      <c r="D80" s="39"/>
-      <c r="E80" s="39"/>
+      <c r="A80" s="35"/>
+      <c r="B80" s="35"/>
+      <c r="C80" s="35"/>
+      <c r="D80" s="35"/>
+      <c r="E80" s="35"/>
     </row>
     <row r="81" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="39"/>
-      <c r="B81" s="39"/>
-      <c r="C81" s="39"/>
-      <c r="D81" s="39"/>
-      <c r="E81" s="39"/>
+      <c r="A81" s="35"/>
+      <c r="B81" s="35"/>
+      <c r="C81" s="35"/>
+      <c r="D81" s="35"/>
+      <c r="E81" s="35"/>
     </row>
     <row r="82" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="39"/>
-      <c r="B82" s="39"/>
-      <c r="C82" s="39"/>
-      <c r="D82" s="39"/>
-      <c r="E82" s="39"/>
+      <c r="A82" s="35"/>
+      <c r="B82" s="35"/>
+      <c r="C82" s="35"/>
+      <c r="D82" s="35"/>
+      <c r="E82" s="35"/>
     </row>
     <row r="83" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="39"/>
-      <c r="B83" s="39"/>
-      <c r="C83" s="39"/>
-      <c r="D83" s="39"/>
-      <c r="E83" s="39"/>
+      <c r="A83" s="35"/>
+      <c r="B83" s="35"/>
+      <c r="C83" s="35"/>
+      <c r="D83" s="35"/>
+      <c r="E83" s="35"/>
     </row>
     <row r="84" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="39"/>
-      <c r="B84" s="39"/>
-      <c r="C84" s="39"/>
-      <c r="D84" s="39"/>
-      <c r="E84" s="39"/>
+      <c r="A84" s="35"/>
+      <c r="B84" s="35"/>
+      <c r="C84" s="35"/>
+      <c r="D84" s="35"/>
+      <c r="E84" s="35"/>
     </row>
     <row r="85" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="39"/>
-      <c r="B85" s="39"/>
-      <c r="C85" s="39"/>
-      <c r="D85" s="39"/>
-      <c r="E85" s="39"/>
+      <c r="A85" s="35"/>
+      <c r="B85" s="35"/>
+      <c r="C85" s="35"/>
+      <c r="D85" s="35"/>
+      <c r="E85" s="35"/>
     </row>
     <row r="86" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="39"/>
-      <c r="B86" s="39"/>
-      <c r="C86" s="39"/>
-      <c r="D86" s="39"/>
-      <c r="E86" s="39"/>
+      <c r="A86" s="35"/>
+      <c r="B86" s="35"/>
+      <c r="C86" s="35"/>
+      <c r="D86" s="35"/>
+      <c r="E86" s="35"/>
     </row>
     <row r="87" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="39"/>
-      <c r="B87" s="39"/>
-      <c r="C87" s="39"/>
-      <c r="D87" s="39"/>
-      <c r="E87" s="39"/>
+      <c r="A87" s="35"/>
+      <c r="B87" s="35"/>
+      <c r="C87" s="35"/>
+      <c r="D87" s="35"/>
+      <c r="E87" s="35"/>
     </row>
     <row r="88" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="39"/>
-      <c r="B88" s="39"/>
-      <c r="C88" s="39"/>
-      <c r="D88" s="39"/>
-      <c r="E88" s="39"/>
+      <c r="A88" s="35"/>
+      <c r="B88" s="35"/>
+      <c r="C88" s="35"/>
+      <c r="D88" s="35"/>
+      <c r="E88" s="35"/>
     </row>
     <row r="89" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="39"/>
-      <c r="B89" s="39"/>
-      <c r="C89" s="39"/>
-      <c r="D89" s="39"/>
-      <c r="E89" s="39"/>
+      <c r="A89" s="35"/>
+      <c r="B89" s="35"/>
+      <c r="C89" s="35"/>
+      <c r="D89" s="35"/>
+      <c r="E89" s="35"/>
     </row>
     <row r="90" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="39"/>
-      <c r="B90" s="39"/>
-      <c r="C90" s="39"/>
-      <c r="D90" s="39"/>
-      <c r="E90" s="39"/>
+      <c r="A90" s="35"/>
+      <c r="B90" s="35"/>
+      <c r="C90" s="35"/>
+      <c r="D90" s="35"/>
+      <c r="E90" s="35"/>
     </row>
     <row r="91" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="39"/>
-      <c r="B91" s="39"/>
-      <c r="C91" s="39"/>
-      <c r="D91" s="39"/>
-      <c r="E91" s="39"/>
+      <c r="A91" s="35"/>
+      <c r="B91" s="35"/>
+      <c r="C91" s="35"/>
+      <c r="D91" s="35"/>
+      <c r="E91" s="35"/>
     </row>
     <row r="92" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="39"/>
-      <c r="B92" s="39"/>
-      <c r="C92" s="39"/>
-      <c r="D92" s="39"/>
-      <c r="E92" s="39"/>
+      <c r="A92" s="35"/>
+      <c r="B92" s="35"/>
+      <c r="C92" s="35"/>
+      <c r="D92" s="35"/>
+      <c r="E92" s="35"/>
     </row>
     <row r="93" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="39"/>
-      <c r="B93" s="39"/>
-      <c r="C93" s="39"/>
-      <c r="D93" s="39"/>
-      <c r="E93" s="39"/>
+      <c r="A93" s="35"/>
+      <c r="B93" s="35"/>
+      <c r="C93" s="35"/>
+      <c r="D93" s="35"/>
+      <c r="E93" s="35"/>
     </row>
     <row r="94" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="39"/>
-      <c r="B94" s="39"/>
-      <c r="C94" s="39"/>
-      <c r="D94" s="39"/>
-      <c r="E94" s="39"/>
+      <c r="A94" s="35"/>
+      <c r="B94" s="35"/>
+      <c r="C94" s="35"/>
+      <c r="D94" s="35"/>
+      <c r="E94" s="35"/>
     </row>
     <row r="95" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="39"/>
-      <c r="B95" s="39"/>
-      <c r="C95" s="39"/>
-      <c r="D95" s="39"/>
-      <c r="E95" s="39"/>
+      <c r="A95" s="35"/>
+      <c r="B95" s="35"/>
+      <c r="C95" s="35"/>
+      <c r="D95" s="35"/>
+      <c r="E95" s="35"/>
     </row>
     <row r="96" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="39"/>
-      <c r="B96" s="39"/>
-      <c r="C96" s="39"/>
-      <c r="D96" s="39"/>
-      <c r="E96" s="39"/>
+      <c r="A96" s="35"/>
+      <c r="B96" s="35"/>
+      <c r="C96" s="35"/>
+      <c r="D96" s="35"/>
+      <c r="E96" s="35"/>
     </row>
     <row r="97" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="39"/>
-      <c r="B97" s="39"/>
-      <c r="C97" s="39"/>
-      <c r="D97" s="39"/>
-      <c r="E97" s="39"/>
+      <c r="A97" s="35"/>
+      <c r="B97" s="35"/>
+      <c r="C97" s="35"/>
+      <c r="D97" s="35"/>
+      <c r="E97" s="35"/>
     </row>
     <row r="98" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="39"/>
-      <c r="B98" s="39"/>
-      <c r="C98" s="39"/>
-      <c r="D98" s="39"/>
-      <c r="E98" s="39"/>
+      <c r="A98" s="35"/>
+      <c r="B98" s="35"/>
+      <c r="C98" s="35"/>
+      <c r="D98" s="35"/>
+      <c r="E98" s="35"/>
     </row>
     <row r="99" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="39"/>
-      <c r="B99" s="39"/>
-      <c r="C99" s="39"/>
-      <c r="D99" s="39"/>
-      <c r="E99" s="39"/>
+      <c r="A99" s="35"/>
+      <c r="B99" s="35"/>
+      <c r="C99" s="35"/>
+      <c r="D99" s="35"/>
+      <c r="E99" s="35"/>
     </row>
     <row r="100" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="39"/>
-      <c r="B100" s="39"/>
-      <c r="C100" s="39"/>
-      <c r="D100" s="39"/>
-      <c r="E100" s="39"/>
+      <c r="A100" s="35"/>
+      <c r="B100" s="35"/>
+      <c r="C100" s="35"/>
+      <c r="D100" s="35"/>
+      <c r="E100" s="35"/>
     </row>
     <row r="101" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="39"/>
-      <c r="B101" s="39"/>
-      <c r="C101" s="39"/>
-      <c r="D101" s="39"/>
-      <c r="E101" s="39"/>
+      <c r="A101" s="35"/>
+      <c r="B101" s="35"/>
+      <c r="C101" s="35"/>
+      <c r="D101" s="35"/>
+      <c r="E101" s="35"/>
     </row>
     <row r="102" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="39"/>
-      <c r="B102" s="39"/>
-      <c r="C102" s="39"/>
-      <c r="D102" s="39"/>
-      <c r="E102" s="39"/>
+      <c r="A102" s="35"/>
+      <c r="B102" s="35"/>
+      <c r="C102" s="35"/>
+      <c r="D102" s="35"/>
+      <c r="E102" s="35"/>
     </row>
     <row r="103" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="39"/>
-      <c r="B103" s="39"/>
-      <c r="C103" s="39"/>
-      <c r="D103" s="39"/>
-      <c r="E103" s="39"/>
+      <c r="A103" s="35"/>
+      <c r="B103" s="35"/>
+      <c r="C103" s="35"/>
+      <c r="D103" s="35"/>
+      <c r="E103" s="35"/>
     </row>
     <row r="104" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="39"/>
-      <c r="B104" s="39"/>
-      <c r="C104" s="39"/>
-      <c r="D104" s="39"/>
-      <c r="E104" s="39"/>
+      <c r="A104" s="35"/>
+      <c r="B104" s="35"/>
+      <c r="C104" s="35"/>
+      <c r="D104" s="35"/>
+      <c r="E104" s="35"/>
     </row>
     <row r="105" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="39"/>
-      <c r="B105" s="39"/>
-      <c r="C105" s="39"/>
-      <c r="D105" s="39"/>
-      <c r="E105" s="39"/>
+      <c r="A105" s="35"/>
+      <c r="B105" s="35"/>
+      <c r="C105" s="35"/>
+      <c r="D105" s="35"/>
+      <c r="E105" s="35"/>
     </row>
     <row r="106" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="39"/>
-      <c r="B106" s="39"/>
-      <c r="C106" s="39"/>
-      <c r="D106" s="39"/>
-      <c r="E106" s="39"/>
+      <c r="A106" s="35"/>
+      <c r="B106" s="35"/>
+      <c r="C106" s="35"/>
+      <c r="D106" s="35"/>
+      <c r="E106" s="35"/>
     </row>
     <row r="107" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="39"/>
-      <c r="B107" s="39"/>
-      <c r="C107" s="39"/>
-      <c r="D107" s="39"/>
-      <c r="E107" s="39"/>
+      <c r="A107" s="35"/>
+      <c r="B107" s="35"/>
+      <c r="C107" s="35"/>
+      <c r="D107" s="35"/>
+      <c r="E107" s="35"/>
     </row>
     <row r="108" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="39"/>
-      <c r="B108" s="39"/>
-      <c r="C108" s="39"/>
-      <c r="D108" s="39"/>
-      <c r="E108" s="39"/>
+      <c r="A108" s="35"/>
+      <c r="B108" s="35"/>
+      <c r="C108" s="35"/>
+      <c r="D108" s="35"/>
+      <c r="E108" s="35"/>
     </row>
     <row r="109" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="39"/>
-      <c r="B109" s="39"/>
-      <c r="C109" s="39"/>
-      <c r="D109" s="39"/>
-      <c r="E109" s="39"/>
+      <c r="A109" s="35"/>
+      <c r="B109" s="35"/>
+      <c r="C109" s="35"/>
+      <c r="D109" s="35"/>
+      <c r="E109" s="35"/>
     </row>
     <row r="110" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="39"/>
-      <c r="B110" s="39"/>
-      <c r="C110" s="39"/>
-      <c r="D110" s="39"/>
-      <c r="E110" s="39"/>
+      <c r="A110" s="35"/>
+      <c r="B110" s="35"/>
+      <c r="C110" s="35"/>
+      <c r="D110" s="35"/>
+      <c r="E110" s="35"/>
     </row>
     <row r="111" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="39"/>
-      <c r="B111" s="39"/>
-      <c r="C111" s="39"/>
-      <c r="D111" s="39"/>
-      <c r="E111" s="39"/>
+      <c r="A111" s="35"/>
+      <c r="B111" s="35"/>
+      <c r="C111" s="35"/>
+      <c r="D111" s="35"/>
+      <c r="E111" s="35"/>
     </row>
     <row r="112" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="39"/>
-      <c r="B112" s="39"/>
-      <c r="C112" s="39"/>
-      <c r="D112" s="39"/>
-      <c r="E112" s="39"/>
+      <c r="A112" s="35"/>
+      <c r="B112" s="35"/>
+      <c r="C112" s="35"/>
+      <c r="D112" s="35"/>
+      <c r="E112" s="35"/>
     </row>
     <row r="113" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="39"/>
-      <c r="B113" s="39"/>
-      <c r="C113" s="39"/>
-      <c r="D113" s="39"/>
-      <c r="E113" s="39"/>
+      <c r="A113" s="35"/>
+      <c r="B113" s="35"/>
+      <c r="C113" s="35"/>
+      <c r="D113" s="35"/>
+      <c r="E113" s="35"/>
     </row>
     <row r="114" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="39"/>
-      <c r="B114" s="39"/>
-      <c r="C114" s="39"/>
-      <c r="D114" s="39"/>
-      <c r="E114" s="39"/>
+      <c r="A114" s="35"/>
+      <c r="B114" s="35"/>
+      <c r="C114" s="35"/>
+      <c r="D114" s="35"/>
+      <c r="E114" s="35"/>
     </row>
     <row r="115" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="39"/>
-      <c r="B115" s="39"/>
-      <c r="C115" s="39"/>
-      <c r="D115" s="39"/>
-      <c r="E115" s="39"/>
+      <c r="A115" s="35"/>
+      <c r="B115" s="35"/>
+      <c r="C115" s="35"/>
+      <c r="D115" s="35"/>
+      <c r="E115" s="35"/>
     </row>
     <row r="116" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="39"/>
-      <c r="B116" s="39"/>
-      <c r="C116" s="39"/>
-      <c r="D116" s="39"/>
-      <c r="E116" s="39"/>
+      <c r="A116" s="35"/>
+      <c r="B116" s="35"/>
+      <c r="C116" s="35"/>
+      <c r="D116" s="35"/>
+      <c r="E116" s="35"/>
     </row>
     <row r="117" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="39"/>
-      <c r="B117" s="39"/>
-      <c r="C117" s="39"/>
-      <c r="D117" s="39"/>
-      <c r="E117" s="39"/>
+      <c r="A117" s="35"/>
+      <c r="B117" s="35"/>
+      <c r="C117" s="35"/>
+      <c r="D117" s="35"/>
+      <c r="E117" s="35"/>
     </row>
     <row r="118" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="39"/>
-      <c r="B118" s="39"/>
-      <c r="C118" s="39"/>
-      <c r="D118" s="39"/>
-      <c r="E118" s="39"/>
+      <c r="A118" s="35"/>
+      <c r="B118" s="35"/>
+      <c r="C118" s="35"/>
+      <c r="D118" s="35"/>
+      <c r="E118" s="35"/>
     </row>
     <row r="119" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="39"/>
-      <c r="B119" s="39"/>
-      <c r="C119" s="39"/>
-      <c r="D119" s="39"/>
-      <c r="E119" s="39"/>
+      <c r="A119" s="35"/>
+      <c r="B119" s="35"/>
+      <c r="C119" s="35"/>
+      <c r="D119" s="35"/>
+      <c r="E119" s="35"/>
     </row>
     <row r="120" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="39"/>
-      <c r="B120" s="39"/>
-      <c r="C120" s="39"/>
-      <c r="D120" s="39"/>
-      <c r="E120" s="39"/>
+      <c r="A120" s="35"/>
+      <c r="B120" s="35"/>
+      <c r="C120" s="35"/>
+      <c r="D120" s="35"/>
+      <c r="E120" s="35"/>
     </row>
     <row r="121" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="39"/>
-      <c r="B121" s="39"/>
-      <c r="C121" s="39"/>
-      <c r="D121" s="39"/>
-      <c r="E121" s="39"/>
+      <c r="A121" s="35"/>
+      <c r="B121" s="35"/>
+      <c r="C121" s="35"/>
+      <c r="D121" s="35"/>
+      <c r="E121" s="35"/>
     </row>
     <row r="122" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="39"/>
-      <c r="B122" s="39"/>
-      <c r="C122" s="39"/>
-      <c r="D122" s="39"/>
-      <c r="E122" s="39"/>
+      <c r="A122" s="35"/>
+      <c r="B122" s="35"/>
+      <c r="C122" s="35"/>
+      <c r="D122" s="35"/>
+      <c r="E122" s="35"/>
     </row>
     <row r="123" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="39"/>
-      <c r="B123" s="39"/>
-      <c r="C123" s="39"/>
-      <c r="D123" s="39"/>
-      <c r="E123" s="39"/>
+      <c r="A123" s="35"/>
+      <c r="B123" s="35"/>
+      <c r="C123" s="35"/>
+      <c r="D123" s="35"/>
+      <c r="E123" s="35"/>
     </row>
     <row r="124" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="39"/>
-      <c r="B124" s="39"/>
-      <c r="C124" s="39"/>
-      <c r="D124" s="39"/>
-      <c r="E124" s="39"/>
+      <c r="A124" s="35"/>
+      <c r="B124" s="35"/>
+      <c r="C124" s="35"/>
+      <c r="D124" s="35"/>
+      <c r="E124" s="35"/>
     </row>
     <row r="125" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="39"/>
-      <c r="B125" s="39"/>
-      <c r="C125" s="39"/>
-      <c r="D125" s="39"/>
-      <c r="E125" s="39"/>
+      <c r="A125" s="35"/>
+      <c r="B125" s="35"/>
+      <c r="C125" s="35"/>
+      <c r="D125" s="35"/>
+      <c r="E125" s="35"/>
     </row>
     <row r="126" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="39"/>
-      <c r="B126" s="39"/>
-      <c r="C126" s="39"/>
-      <c r="D126" s="39"/>
-      <c r="E126" s="39"/>
+      <c r="A126" s="35"/>
+      <c r="B126" s="35"/>
+      <c r="C126" s="35"/>
+      <c r="D126" s="35"/>
+      <c r="E126" s="35"/>
     </row>
     <row r="127" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="39"/>
-      <c r="B127" s="39"/>
-      <c r="C127" s="39"/>
-      <c r="D127" s="39"/>
-      <c r="E127" s="39"/>
+      <c r="A127" s="35"/>
+      <c r="B127" s="35"/>
+      <c r="C127" s="35"/>
+      <c r="D127" s="35"/>
+      <c r="E127" s="35"/>
     </row>
     <row r="128" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="39"/>
-      <c r="B128" s="39"/>
-      <c r="C128" s="39"/>
-      <c r="D128" s="39"/>
-      <c r="E128" s="39"/>
+      <c r="A128" s="35"/>
+      <c r="B128" s="35"/>
+      <c r="C128" s="35"/>
+      <c r="D128" s="35"/>
+      <c r="E128" s="35"/>
     </row>
     <row r="129" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="39"/>
-      <c r="B129" s="39"/>
-      <c r="C129" s="39"/>
-      <c r="D129" s="39"/>
-      <c r="E129" s="39"/>
+      <c r="A129" s="35"/>
+      <c r="B129" s="35"/>
+      <c r="C129" s="35"/>
+      <c r="D129" s="35"/>
+      <c r="E129" s="35"/>
     </row>
     <row r="130" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="39"/>
-      <c r="B130" s="39"/>
-      <c r="C130" s="39"/>
-      <c r="D130" s="39"/>
-      <c r="E130" s="39"/>
+      <c r="A130" s="35"/>
+      <c r="B130" s="35"/>
+      <c r="C130" s="35"/>
+      <c r="D130" s="35"/>
+      <c r="E130" s="35"/>
     </row>
     <row r="131" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="39"/>
-      <c r="B131" s="39"/>
-      <c r="C131" s="39"/>
-      <c r="D131" s="39"/>
-      <c r="E131" s="39"/>
+      <c r="A131" s="35"/>
+      <c r="B131" s="35"/>
+      <c r="C131" s="35"/>
+      <c r="D131" s="35"/>
+      <c r="E131" s="35"/>
     </row>
     <row r="132" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="39"/>
-      <c r="B132" s="39"/>
-      <c r="C132" s="39"/>
-      <c r="D132" s="39"/>
-      <c r="E132" s="39"/>
+      <c r="A132" s="35"/>
+      <c r="B132" s="35"/>
+      <c r="C132" s="35"/>
+      <c r="D132" s="35"/>
+      <c r="E132" s="35"/>
     </row>
     <row r="133" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="39"/>
-      <c r="B133" s="39"/>
-      <c r="C133" s="39"/>
-      <c r="D133" s="39"/>
-      <c r="E133" s="39"/>
+      <c r="A133" s="35"/>
+      <c r="B133" s="35"/>
+      <c r="C133" s="35"/>
+      <c r="D133" s="35"/>
+      <c r="E133" s="35"/>
     </row>
     <row r="134" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="39"/>
-      <c r="B134" s="39"/>
-      <c r="C134" s="39"/>
-      <c r="D134" s="39"/>
-      <c r="E134" s="39"/>
+      <c r="A134" s="35"/>
+      <c r="B134" s="35"/>
+      <c r="C134" s="35"/>
+      <c r="D134" s="35"/>
+      <c r="E134" s="35"/>
     </row>
     <row r="135" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="39"/>
-      <c r="B135" s="39"/>
-      <c r="C135" s="39"/>
-      <c r="D135" s="39"/>
-      <c r="E135" s="39"/>
+      <c r="A135" s="35"/>
+      <c r="B135" s="35"/>
+      <c r="C135" s="35"/>
+      <c r="D135" s="35"/>
+      <c r="E135" s="35"/>
     </row>
     <row r="136" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A136" s="39"/>
-      <c r="B136" s="39"/>
-      <c r="C136" s="39"/>
-      <c r="D136" s="39"/>
-      <c r="E136" s="39"/>
+      <c r="A136" s="35"/>
+      <c r="B136" s="35"/>
+      <c r="C136" s="35"/>
+      <c r="D136" s="35"/>
+      <c r="E136" s="35"/>
     </row>
     <row r="137" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A137" s="39"/>
-      <c r="B137" s="39"/>
-      <c r="C137" s="39"/>
-      <c r="D137" s="39"/>
-      <c r="E137" s="39"/>
+      <c r="A137" s="35"/>
+      <c r="B137" s="35"/>
+      <c r="C137" s="35"/>
+      <c r="D137" s="35"/>
+      <c r="E137" s="35"/>
     </row>
     <row r="138" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A138" s="39"/>
-      <c r="B138" s="39"/>
-      <c r="C138" s="39"/>
-      <c r="D138" s="39"/>
-      <c r="E138" s="39"/>
+      <c r="A138" s="35"/>
+      <c r="B138" s="35"/>
+      <c r="C138" s="35"/>
+      <c r="D138" s="35"/>
+      <c r="E138" s="35"/>
     </row>
     <row r="139" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A139" s="39"/>
-      <c r="B139" s="39"/>
-      <c r="C139" s="39"/>
-      <c r="D139" s="39"/>
-      <c r="E139" s="39"/>
+      <c r="A139" s="35"/>
+      <c r="B139" s="35"/>
+      <c r="C139" s="35"/>
+      <c r="D139" s="35"/>
+      <c r="E139" s="35"/>
     </row>
     <row r="140" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A140" s="39"/>
-      <c r="B140" s="39"/>
-      <c r="C140" s="39"/>
-      <c r="D140" s="39"/>
-      <c r="E140" s="39"/>
+      <c r="A140" s="35"/>
+      <c r="B140" s="35"/>
+      <c r="C140" s="35"/>
+      <c r="D140" s="35"/>
+      <c r="E140" s="35"/>
     </row>
     <row r="141" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A141" s="39"/>
-      <c r="B141" s="39"/>
-      <c r="C141" s="39"/>
-      <c r="D141" s="39"/>
-      <c r="E141" s="39"/>
+      <c r="A141" s="35"/>
+      <c r="B141" s="35"/>
+      <c r="C141" s="35"/>
+      <c r="D141" s="35"/>
+      <c r="E141" s="35"/>
     </row>
     <row r="142" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A142" s="39"/>
-      <c r="B142" s="39"/>
-      <c r="C142" s="39"/>
-      <c r="D142" s="39"/>
-      <c r="E142" s="39"/>
+      <c r="A142" s="35"/>
+      <c r="B142" s="35"/>
+      <c r="C142" s="35"/>
+      <c r="D142" s="35"/>
+      <c r="E142" s="35"/>
     </row>
     <row r="143" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A143" s="39"/>
-      <c r="B143" s="39"/>
-      <c r="C143" s="39"/>
-      <c r="D143" s="39"/>
-      <c r="E143" s="39"/>
+      <c r="A143" s="35"/>
+      <c r="B143" s="35"/>
+      <c r="C143" s="35"/>
+      <c r="D143" s="35"/>
+      <c r="E143" s="35"/>
     </row>
     <row r="144" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A144" s="39"/>
-      <c r="B144" s="39"/>
-      <c r="C144" s="39"/>
-      <c r="D144" s="39"/>
-      <c r="E144" s="39"/>
+      <c r="A144" s="35"/>
+      <c r="B144" s="35"/>
+      <c r="C144" s="35"/>
+      <c r="D144" s="35"/>
+      <c r="E144" s="35"/>
     </row>
     <row r="145" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A145" s="39"/>
-      <c r="B145" s="39"/>
-      <c r="C145" s="39"/>
-      <c r="D145" s="39"/>
-      <c r="E145" s="39"/>
+      <c r="A145" s="35"/>
+      <c r="B145" s="35"/>
+      <c r="C145" s="35"/>
+      <c r="D145" s="35"/>
+      <c r="E145" s="35"/>
     </row>
     <row r="146" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A146" s="39"/>
-      <c r="B146" s="39"/>
-      <c r="C146" s="39"/>
-      <c r="D146" s="39"/>
-      <c r="E146" s="39"/>
+      <c r="A146" s="35"/>
+      <c r="B146" s="35"/>
+      <c r="C146" s="35"/>
+      <c r="D146" s="35"/>
+      <c r="E146" s="35"/>
     </row>
     <row r="147" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A147" s="39"/>
-      <c r="B147" s="39"/>
-      <c r="C147" s="39"/>
-      <c r="D147" s="39"/>
-      <c r="E147" s="39"/>
+      <c r="A147" s="35"/>
+      <c r="B147" s="35"/>
+      <c r="C147" s="35"/>
+      <c r="D147" s="35"/>
+      <c r="E147" s="35"/>
     </row>
     <row r="148" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A148" s="39"/>
-      <c r="B148" s="39"/>
-      <c r="C148" s="39"/>
-      <c r="D148" s="39"/>
-      <c r="E148" s="39"/>
+      <c r="A148" s="35"/>
+      <c r="B148" s="35"/>
+      <c r="C148" s="35"/>
+      <c r="D148" s="35"/>
+      <c r="E148" s="35"/>
     </row>
     <row r="149" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A149" s="39"/>
-      <c r="B149" s="39"/>
-      <c r="C149" s="39"/>
-      <c r="D149" s="39"/>
-      <c r="E149" s="39"/>
+      <c r="A149" s="35"/>
+      <c r="B149" s="35"/>
+      <c r="C149" s="35"/>
+      <c r="D149" s="35"/>
+      <c r="E149" s="35"/>
     </row>
     <row r="150" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A150" s="39"/>
-      <c r="B150" s="39"/>
-      <c r="C150" s="39"/>
-      <c r="D150" s="39"/>
-      <c r="E150" s="39"/>
+      <c r="A150" s="35"/>
+      <c r="B150" s="35"/>
+      <c r="C150" s="35"/>
+      <c r="D150" s="35"/>
+      <c r="E150" s="35"/>
     </row>
     <row r="151" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A151" s="39"/>
-      <c r="B151" s="39"/>
-      <c r="C151" s="39"/>
-      <c r="D151" s="39"/>
-      <c r="E151" s="39"/>
+      <c r="A151" s="35"/>
+      <c r="B151" s="35"/>
+      <c r="C151" s="35"/>
+      <c r="D151" s="35"/>
+      <c r="E151" s="35"/>
     </row>
     <row r="152" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A152" s="39"/>
-      <c r="B152" s="39"/>
-      <c r="C152" s="39"/>
-      <c r="D152" s="39"/>
-      <c r="E152" s="39"/>
+      <c r="A152" s="35"/>
+      <c r="B152" s="35"/>
+      <c r="C152" s="35"/>
+      <c r="D152" s="35"/>
+      <c r="E152" s="35"/>
     </row>
     <row r="153" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A153" s="39"/>
-      <c r="B153" s="39"/>
-      <c r="C153" s="39"/>
-      <c r="D153" s="39"/>
-      <c r="E153" s="39"/>
+      <c r="A153" s="35"/>
+      <c r="B153" s="35"/>
+      <c r="C153" s="35"/>
+      <c r="D153" s="35"/>
+      <c r="E153" s="35"/>
     </row>
     <row r="154" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A154" s="39"/>
-      <c r="B154" s="39"/>
-      <c r="C154" s="39"/>
-      <c r="D154" s="39"/>
-      <c r="E154" s="39"/>
+      <c r="A154" s="35"/>
+      <c r="B154" s="35"/>
+      <c r="C154" s="35"/>
+      <c r="D154" s="35"/>
+      <c r="E154" s="35"/>
     </row>
     <row r="155" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A155" s="39"/>
-      <c r="B155" s="39"/>
-      <c r="C155" s="39"/>
-      <c r="D155" s="39"/>
-      <c r="E155" s="39"/>
+      <c r="A155" s="35"/>
+      <c r="B155" s="35"/>
+      <c r="C155" s="35"/>
+      <c r="D155" s="35"/>
+      <c r="E155" s="35"/>
     </row>
     <row r="156" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A156" s="39"/>
-      <c r="B156" s="39"/>
-      <c r="C156" s="39"/>
-      <c r="D156" s="39"/>
-      <c r="E156" s="39"/>
+      <c r="A156" s="35"/>
+      <c r="B156" s="35"/>
+      <c r="C156" s="35"/>
+      <c r="D156" s="35"/>
+      <c r="E156" s="35"/>
     </row>
     <row r="157" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A157" s="39"/>
-      <c r="B157" s="39"/>
-      <c r="C157" s="39"/>
-      <c r="D157" s="39"/>
-      <c r="E157" s="39"/>
+      <c r="A157" s="35"/>
+      <c r="B157" s="35"/>
+      <c r="C157" s="35"/>
+      <c r="D157" s="35"/>
+      <c r="E157" s="35"/>
     </row>
     <row r="158" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A158" s="39"/>
-      <c r="B158" s="39"/>
-      <c r="C158" s="39"/>
-      <c r="D158" s="39"/>
-      <c r="E158" s="39"/>
+      <c r="A158" s="35"/>
+      <c r="B158" s="35"/>
+      <c r="C158" s="35"/>
+      <c r="D158" s="35"/>
+      <c r="E158" s="35"/>
     </row>
     <row r="159" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A159" s="39"/>
-      <c r="B159" s="39"/>
-      <c r="C159" s="39"/>
-      <c r="D159" s="39"/>
-      <c r="E159" s="39"/>
+      <c r="A159" s="35"/>
+      <c r="B159" s="35"/>
+      <c r="C159" s="35"/>
+      <c r="D159" s="35"/>
+      <c r="E159" s="35"/>
     </row>
     <row r="160" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A160" s="39"/>
-      <c r="B160" s="39"/>
-      <c r="C160" s="39"/>
-      <c r="D160" s="39"/>
-      <c r="E160" s="39"/>
+      <c r="A160" s="35"/>
+      <c r="B160" s="35"/>
+      <c r="C160" s="35"/>
+      <c r="D160" s="35"/>
+      <c r="E160" s="35"/>
     </row>
     <row r="161" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A161" s="39"/>
-      <c r="B161" s="39"/>
-      <c r="C161" s="39"/>
-      <c r="D161" s="39"/>
-      <c r="E161" s="39"/>
+      <c r="A161" s="35"/>
+      <c r="B161" s="35"/>
+      <c r="C161" s="35"/>
+      <c r="D161" s="35"/>
+      <c r="E161" s="35"/>
     </row>
     <row r="162" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A162" s="39"/>
-      <c r="B162" s="39"/>
-      <c r="C162" s="39"/>
-      <c r="D162" s="39"/>
-      <c r="E162" s="39"/>
+      <c r="A162" s="35"/>
+      <c r="B162" s="35"/>
+      <c r="C162" s="35"/>
+      <c r="D162" s="35"/>
+      <c r="E162" s="35"/>
     </row>
     <row r="163" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A163" s="39"/>
-      <c r="B163" s="39"/>
-      <c r="C163" s="39"/>
-      <c r="D163" s="39"/>
-      <c r="E163" s="39"/>
+      <c r="A163" s="35"/>
+      <c r="B163" s="35"/>
+      <c r="C163" s="35"/>
+      <c r="D163" s="35"/>
+      <c r="E163" s="35"/>
     </row>
     <row r="164" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A164" s="39"/>
-      <c r="B164" s="39"/>
-      <c r="C164" s="39"/>
-      <c r="D164" s="39"/>
-      <c r="E164" s="39"/>
+      <c r="A164" s="35"/>
+      <c r="B164" s="35"/>
+      <c r="C164" s="35"/>
+      <c r="D164" s="35"/>
+      <c r="E164" s="35"/>
     </row>
     <row r="165" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A165" s="39"/>
-      <c r="B165" s="39"/>
-      <c r="C165" s="39"/>
-      <c r="D165" s="39"/>
-      <c r="E165" s="39"/>
+      <c r="A165" s="35"/>
+      <c r="B165" s="35"/>
+      <c r="C165" s="35"/>
+      <c r="D165" s="35"/>
+      <c r="E165" s="35"/>
     </row>
     <row r="166" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A166" s="39"/>
-      <c r="B166" s="39"/>
-      <c r="C166" s="39"/>
-      <c r="D166" s="39"/>
-      <c r="E166" s="39"/>
+      <c r="A166" s="35"/>
+      <c r="B166" s="35"/>
+      <c r="C166" s="35"/>
+      <c r="D166" s="35"/>
+      <c r="E166" s="35"/>
     </row>
     <row r="167" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A167" s="39"/>
-      <c r="B167" s="39"/>
-      <c r="C167" s="39"/>
-      <c r="D167" s="39"/>
-      <c r="E167" s="39"/>
+      <c r="A167" s="35"/>
+      <c r="B167" s="35"/>
+      <c r="C167" s="35"/>
+      <c r="D167" s="35"/>
+      <c r="E167" s="35"/>
     </row>
     <row r="168" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A168" s="39"/>
-      <c r="B168" s="39"/>
-      <c r="C168" s="39"/>
-      <c r="D168" s="39"/>
-      <c r="E168" s="39"/>
+      <c r="A168" s="35"/>
+      <c r="B168" s="35"/>
+      <c r="C168" s="35"/>
+      <c r="D168" s="35"/>
+      <c r="E168" s="35"/>
     </row>
     <row r="169" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A169" s="39"/>
-      <c r="B169" s="39"/>
-      <c r="C169" s="39"/>
-      <c r="D169" s="39"/>
-      <c r="E169" s="39"/>
+      <c r="A169" s="35"/>
+      <c r="B169" s="35"/>
+      <c r="C169" s="35"/>
+      <c r="D169" s="35"/>
+      <c r="E169" s="35"/>
     </row>
     <row r="170" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A170" s="39"/>
-      <c r="B170" s="39"/>
-      <c r="C170" s="39"/>
-      <c r="D170" s="39"/>
-      <c r="E170" s="39"/>
+      <c r="A170" s="35"/>
+      <c r="B170" s="35"/>
+      <c r="C170" s="35"/>
+      <c r="D170" s="35"/>
+      <c r="E170" s="35"/>
     </row>
     <row r="171" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A171" s="39"/>
-      <c r="B171" s="39"/>
-      <c r="C171" s="39"/>
-      <c r="D171" s="39"/>
-      <c r="E171" s="39"/>
+      <c r="A171" s="35"/>
+      <c r="B171" s="35"/>
+      <c r="C171" s="35"/>
+      <c r="D171" s="35"/>
+      <c r="E171" s="35"/>
     </row>
     <row r="172" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A172" s="39"/>
-      <c r="B172" s="39"/>
-      <c r="C172" s="39"/>
-      <c r="D172" s="39"/>
-      <c r="E172" s="39"/>
+      <c r="A172" s="35"/>
+      <c r="B172" s="35"/>
+      <c r="C172" s="35"/>
+      <c r="D172" s="35"/>
+      <c r="E172" s="35"/>
     </row>
     <row r="173" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A173" s="39"/>
-      <c r="B173" s="39"/>
-      <c r="C173" s="39"/>
-      <c r="D173" s="39"/>
-      <c r="E173" s="39"/>
+      <c r="A173" s="35"/>
+      <c r="B173" s="35"/>
+      <c r="C173" s="35"/>
+      <c r="D173" s="35"/>
+      <c r="E173" s="35"/>
     </row>
     <row r="174" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A174" s="39"/>
-      <c r="B174" s="39"/>
-      <c r="C174" s="39"/>
-      <c r="D174" s="39"/>
-      <c r="E174" s="39"/>
+      <c r="A174" s="35"/>
+      <c r="B174" s="35"/>
+      <c r="C174" s="35"/>
+      <c r="D174" s="35"/>
+      <c r="E174" s="35"/>
     </row>
     <row r="175" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A175" s="39"/>
-      <c r="B175" s="39"/>
-      <c r="C175" s="39"/>
-      <c r="D175" s="39"/>
-      <c r="E175" s="39"/>
+      <c r="A175" s="35"/>
+      <c r="B175" s="35"/>
+      <c r="C175" s="35"/>
+      <c r="D175" s="35"/>
+      <c r="E175" s="35"/>
     </row>
     <row r="176" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A176" s="39"/>
-      <c r="B176" s="39"/>
-      <c r="C176" s="39"/>
-      <c r="D176" s="39"/>
-      <c r="E176" s="39"/>
+      <c r="A176" s="35"/>
+      <c r="B176" s="35"/>
+      <c r="C176" s="35"/>
+      <c r="D176" s="35"/>
+      <c r="E176" s="35"/>
     </row>
     <row r="177" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A177" s="39"/>
-      <c r="B177" s="39"/>
-      <c r="C177" s="39"/>
-      <c r="D177" s="39"/>
-      <c r="E177" s="39"/>
+      <c r="A177" s="35"/>
+      <c r="B177" s="35"/>
+      <c r="C177" s="35"/>
+      <c r="D177" s="35"/>
+      <c r="E177" s="35"/>
     </row>
     <row r="178" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A178" s="39"/>
-      <c r="B178" s="39"/>
-      <c r="C178" s="39"/>
-      <c r="D178" s="39"/>
-      <c r="E178" s="39"/>
+      <c r="A178" s="35"/>
+      <c r="B178" s="35"/>
+      <c r="C178" s="35"/>
+      <c r="D178" s="35"/>
+      <c r="E178" s="35"/>
     </row>
     <row r="179" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A179" s="39"/>
-      <c r="B179" s="39"/>
-      <c r="C179" s="39"/>
-      <c r="D179" s="39"/>
-      <c r="E179" s="39"/>
+      <c r="A179" s="35"/>
+      <c r="B179" s="35"/>
+      <c r="C179" s="35"/>
+      <c r="D179" s="35"/>
+      <c r="E179" s="35"/>
     </row>
     <row r="180" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A180" s="39"/>
-      <c r="B180" s="39"/>
-      <c r="C180" s="39"/>
-      <c r="D180" s="39"/>
-      <c r="E180" s="39"/>
+      <c r="A180" s="35"/>
+      <c r="B180" s="35"/>
+      <c r="C180" s="35"/>
+      <c r="D180" s="35"/>
+      <c r="E180" s="35"/>
     </row>
     <row r="181" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A181" s="39"/>
-      <c r="B181" s="39"/>
-      <c r="C181" s="39"/>
-      <c r="D181" s="39"/>
-      <c r="E181" s="39"/>
+      <c r="A181" s="35"/>
+      <c r="B181" s="35"/>
+      <c r="C181" s="35"/>
+      <c r="D181" s="35"/>
+      <c r="E181" s="35"/>
     </row>
     <row r="182" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A182" s="39"/>
-      <c r="B182" s="39"/>
-      <c r="C182" s="39"/>
-      <c r="D182" s="39"/>
-      <c r="E182" s="39"/>
+      <c r="A182" s="35"/>
+      <c r="B182" s="35"/>
+      <c r="C182" s="35"/>
+      <c r="D182" s="35"/>
+      <c r="E182" s="35"/>
     </row>
     <row r="183" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A183" s="39"/>
-      <c r="B183" s="39"/>
-      <c r="C183" s="39"/>
-      <c r="D183" s="39"/>
-      <c r="E183" s="39"/>
+      <c r="A183" s="35"/>
+      <c r="B183" s="35"/>
+      <c r="C183" s="35"/>
+      <c r="D183" s="35"/>
+      <c r="E183" s="35"/>
     </row>
     <row r="184" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A184" s="39"/>
-      <c r="B184" s="39"/>
-      <c r="C184" s="39"/>
-      <c r="D184" s="39"/>
-      <c r="E184" s="39"/>
+      <c r="A184" s="35"/>
+      <c r="B184" s="35"/>
+      <c r="C184" s="35"/>
+      <c r="D184" s="35"/>
+      <c r="E184" s="35"/>
     </row>
     <row r="185" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A185" s="39"/>
-      <c r="B185" s="39"/>
-      <c r="C185" s="39"/>
-      <c r="D185" s="39"/>
-      <c r="E185" s="39"/>
+      <c r="A185" s="35"/>
+      <c r="B185" s="35"/>
+      <c r="C185" s="35"/>
+      <c r="D185" s="35"/>
+      <c r="E185" s="35"/>
     </row>
     <row r="186" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A186" s="39"/>
-      <c r="B186" s="39"/>
-      <c r="C186" s="39"/>
-      <c r="D186" s="39"/>
-      <c r="E186" s="39"/>
+      <c r="A186" s="35"/>
+      <c r="B186" s="35"/>
+      <c r="C186" s="35"/>
+      <c r="D186" s="35"/>
+      <c r="E186" s="35"/>
     </row>
     <row r="187" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A187" s="39"/>
-      <c r="B187" s="39"/>
-      <c r="C187" s="39"/>
-      <c r="D187" s="39"/>
-      <c r="E187" s="39"/>
+      <c r="A187" s="35"/>
+      <c r="B187" s="35"/>
+      <c r="C187" s="35"/>
+      <c r="D187" s="35"/>
+      <c r="E187" s="35"/>
     </row>
     <row r="188" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A188" s="39"/>
-      <c r="B188" s="39"/>
-      <c r="C188" s="39"/>
-      <c r="D188" s="39"/>
-      <c r="E188" s="39"/>
+      <c r="A188" s="35"/>
+      <c r="B188" s="35"/>
+      <c r="C188" s="35"/>
+      <c r="D188" s="35"/>
+      <c r="E188" s="35"/>
     </row>
     <row r="189" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A189" s="39"/>
-      <c r="B189" s="39"/>
-      <c r="C189" s="39"/>
-      <c r="D189" s="39"/>
-      <c r="E189" s="39"/>
+      <c r="A189" s="35"/>
+      <c r="B189" s="35"/>
+      <c r="C189" s="35"/>
+      <c r="D189" s="35"/>
+      <c r="E189" s="35"/>
     </row>
     <row r="190" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A190" s="39"/>
-      <c r="B190" s="39"/>
-      <c r="C190" s="39"/>
-      <c r="D190" s="39"/>
-      <c r="E190" s="39"/>
+      <c r="A190" s="35"/>
+      <c r="B190" s="35"/>
+      <c r="C190" s="35"/>
+      <c r="D190" s="35"/>
+      <c r="E190" s="35"/>
     </row>
     <row r="191" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A191" s="39"/>
-      <c r="B191" s="39"/>
-      <c r="C191" s="39"/>
-      <c r="D191" s="39"/>
-      <c r="E191" s="39"/>
+      <c r="A191" s="35"/>
+      <c r="B191" s="35"/>
+      <c r="C191" s="35"/>
+      <c r="D191" s="35"/>
+      <c r="E191" s="35"/>
     </row>
     <row r="192" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A192" s="39"/>
-      <c r="B192" s="39"/>
-      <c r="C192" s="39"/>
-      <c r="D192" s="39"/>
-      <c r="E192" s="39"/>
+      <c r="A192" s="35"/>
+      <c r="B192" s="35"/>
+      <c r="C192" s="35"/>
+      <c r="D192" s="35"/>
+      <c r="E192" s="35"/>
     </row>
     <row r="193" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A193" s="39"/>
-      <c r="B193" s="39"/>
-      <c r="C193" s="39"/>
-      <c r="D193" s="39"/>
-      <c r="E193" s="39"/>
+      <c r="A193" s="35"/>
+      <c r="B193" s="35"/>
+      <c r="C193" s="35"/>
+      <c r="D193" s="35"/>
+      <c r="E193" s="35"/>
     </row>
     <row r="194" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A194" s="39"/>
-      <c r="B194" s="39"/>
-      <c r="C194" s="39"/>
-      <c r="D194" s="39"/>
-      <c r="E194" s="39"/>
+      <c r="A194" s="35"/>
+      <c r="B194" s="35"/>
+      <c r="C194" s="35"/>
+      <c r="D194" s="35"/>
+      <c r="E194" s="35"/>
     </row>
     <row r="195" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A195" s="39"/>
-      <c r="B195" s="39"/>
-      <c r="C195" s="39"/>
-      <c r="D195" s="39"/>
-      <c r="E195" s="39"/>
+      <c r="A195" s="35"/>
+      <c r="B195" s="35"/>
+      <c r="C195" s="35"/>
+      <c r="D195" s="35"/>
+      <c r="E195" s="35"/>
     </row>
     <row r="196" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A196" s="39"/>
-      <c r="B196" s="39"/>
-      <c r="C196" s="39"/>
-      <c r="D196" s="39"/>
-      <c r="E196" s="39"/>
+      <c r="A196" s="35"/>
+      <c r="B196" s="35"/>
+      <c r="C196" s="35"/>
+      <c r="D196" s="35"/>
+      <c r="E196" s="35"/>
     </row>
     <row r="197" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A197" s="39"/>
-      <c r="B197" s="39"/>
-      <c r="C197" s="39"/>
-      <c r="D197" s="39"/>
-      <c r="E197" s="39"/>
+      <c r="A197" s="35"/>
+      <c r="B197" s="35"/>
+      <c r="C197" s="35"/>
+      <c r="D197" s="35"/>
+      <c r="E197" s="35"/>
     </row>
     <row r="198" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A198" s="39"/>
-      <c r="B198" s="39"/>
-      <c r="C198" s="39"/>
-      <c r="D198" s="39"/>
-      <c r="E198" s="39"/>
+      <c r="A198" s="35"/>
+      <c r="B198" s="35"/>
+      <c r="C198" s="35"/>
+      <c r="D198" s="35"/>
+      <c r="E198" s="35"/>
     </row>
     <row r="199" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A199" s="39"/>
-      <c r="B199" s="39"/>
-      <c r="C199" s="39"/>
-      <c r="D199" s="39"/>
-      <c r="E199" s="39"/>
+      <c r="A199" s="35"/>
+      <c r="B199" s="35"/>
+      <c r="C199" s="35"/>
+      <c r="D199" s="35"/>
+      <c r="E199" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -7679,65 +7573,65 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C5"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.25" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="48" style="14" customWidth="1"/>
-    <col min="3" max="3" width="40.5" style="13" customWidth="1"/>
-    <col min="4" max="16384" width="12.25" style="13"/>
+    <col min="1" max="1" width="11.625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="48" style="13" customWidth="1"/>
+    <col min="3" max="3" width="40.5" style="12" customWidth="1"/>
+    <col min="4" max="16384" width="12.25" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="55" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
+      <c r="A1" s="61" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
     </row>
     <row r="2" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="D2" s="27"/>
+      <c r="C2" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="23"/>
     </row>
     <row r="3" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="68" t="s">
+      <c r="A3" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="53" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="23"/>
+    </row>
+    <row r="4" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="23"/>
+    </row>
+    <row r="5" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="D3" s="27"/>
-    </row>
-    <row r="4" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" s="69" t="s">
-        <v>79</v>
-      </c>
-      <c r="D4" s="27"/>
-    </row>
-    <row r="5" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="14" t="s">
+      <c r="B5" s="54" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="70" t="s">
-        <v>131</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="D5" s="27"/>
+      <c r="D5" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>